<commit_message>
finalizado geração de arquivos com a analise dos modelos
</commit_message>
<xml_diff>
--- a/relatorio_analise_vulnerabilidade - llama-3.3-70b-versatile.xlsx
+++ b/relatorio_analise_vulnerabilidade - llama-3.3-70b-versatile.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C127"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,7 +524,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>vulnerability: NO | vulnerability type: N/A | vulnerability name: N/A | explanation: The provided code snippet is an abstract class extending HttpServlet and overrides several HTTP method handlers (doTrace, doHead, doPost, doDelete, doPut) but does not contain any implementation that could introduce a security vulnerability. The methods are empty, and there are no signs of user input being processed or stored in an insecure manner. Without any actual implementation or usage of potentially vulnerable functions, this code does not appear to be subject to any security vulnerabilities based on the given information.</t>
+          <t>vulnerability: NO | vulnerability type: N/A | vulnerability name: N/A | explanation: The provided code snippet is an abstract class extending HttpServlet and overrides several HTTP method handling functions, but it does not contain any apparent security vulnerabilities as it does not handle any user input or perform any operations that could potentially lead to security issues.</t>
         </is>
       </c>
     </row>
@@ -558,12 +558,33 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.aliasing;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Aliasing1 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+String str = name;
+PrintWriter writer = resp.getWriter();
+writer.println(str);
+}
+public String getDescription() {
+return "simple test of field assignment";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100063, Requested 287. Please try again in 5m3.166s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user-input data (the "name" parameter from the HTTP request) to the response without any validation or sanitization, making it vulnerable to Cross-Site Scripting (XSS) attacks.</t>
         </is>
       </c>
     </row>
@@ -575,12 +596,34 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.aliasing;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Aliasing2 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+String str = "abc";
+name = str;
+PrintWriter writer = resp.getWriter();
+writer.println(str);
+}
+public String getDescription() {
+return "simple aliasing false positive";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100063, Requested 290. Please try again in 5m5.666s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: NO | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet provided does not contain any apparent security vulnerabilities. Although it involves user input from the HttpServletRequest, the input is not used in a way that could lead to security issues such as SQL injection or cross-site scripting (XSS), as the input is immediately reassigned to a static string "abc" before any output or further processing. The output to the HttpServletResponse is a fixed string "abc", which does not depend on the user's input, thus preventing any potential XSS vulnerability.</t>
         </is>
       </c>
     </row>
@@ -592,12 +635,36 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.aliasing;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Aliasing3 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+String[] a = new String[10];
+String str = a[5];
+a[5] = name;
+name = str;
+PrintWriter writer = resp.getWriter();
+writer.println(str);
+}
+public String getDescription() {
+return "simple aliasing of an array element";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100063, Requested 302. Please try again in 5m15.932s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it is vulnerable to a reflected cross-site scripting (XSS) attack. The 'name' parameter from the HTTP request is stored in the 'a' array and then assigned to the 'name' variable, but initially, the 'str' variable is assigned the value of 'a[5]', which is null. Then 'a[5]' is updated with the 'name' parameter, but 'str' still holds the initial null value. However, if the code was modified to directly use the 'name' variable or 'a[5]' after the update, it would be vulnerable to XSS. In the current implementation, since 'str' is used, which holds the initial null value, it does not pose an immediate XSS risk, but the overall handling of user input is still insecure.</t>
         </is>
       </c>
     </row>
@@ -609,12 +676,37 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.aliasing;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Aliasing4 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+Object o1 = name;
+Object o2 = name.concat("abc");
+Object o3 = "anc";
+PrintWriter writer = resp.getWriter();
+writer.println(o1);
+writer.println(o2);
+writer.println(o3);
+}
+public String getDescription() {
+return "simple aliasing with casts";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100063, Requested 308. Please try again in 5m21.026s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user-input data (the "name" parameter) to the response without any validation or sanitization, making it vulnerable to Cross-Site Scripting (XSS) attacks. An attacker could inject malicious JavaScript code as the "name" parameter, which would then be executed by the browser, potentially leading to unauthorized actions or data theft.</t>
         </is>
       </c>
     </row>
@@ -626,12 +718,39 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.aliasing;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.ServletRequest;
+import javax.servlet.ServletResponse;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Aliasing5 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+StringBuffer buf = new StringBuffer("abc");
+foo(buf, buf, resp, req);
+}
+void foo(StringBuffer buf, StringBuffer buf2, ServletResponse resp, ServletRequest req) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+buf.append(name);
+PrintWriter writer = resp.getWriter();
+writer.println(buf2.toString());
+}
+public String getDescription() {
+return "interprocedural argument aliasing";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100063, Requested 354. Please try again in 6m0.676999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it is vulnerable to a Cross-Site Scripting (XSS) attack. The 'name' parameter from the request is directly appended to the StringBuffer 'buf' and then 'buf2' (which is an alias for 'buf') is printed to the response. If an attacker injects malicious JavaScript code as the 'name' parameter, it will be executed when the response is rendered, potentially leading to unauthorized actions or data theft.</t>
         </is>
       </c>
     </row>
@@ -643,12 +762,44 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.aliasing;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Aliasing6 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String[] names = req.getParameterValues(FIELD_NAME);
+Object
+o1, o2, o3, o4, o5, o6, o7, o8, o9, o10, o11, o12, o13, o14, o15, o16, o17, o18, o19, o20,
+o21, o22, o23, o24, o25, o26, o27, o28, o29, o30, o31, o32, o33, o34, o35, o36, o37, o38, o39, o40;
+o1 = o2 = o3 = o4 = o5 = o6 = o7 = o8 = o9 = o10 = o11 = o12 = o13 = o14 = o15 = o16 = o17 = o18 = o19 = o20 =
+o21 = o22 = o23 = o24 = o25 = o26 = o27 = o28 = o29 = o30 = o31 = o32 = o33 = o34 = o35 = o36 = o37 = o38 = o39 = o40 =
+names[0];
+PrintWriter writer = resp.getWriter();
+writer.println(o1);
+writer.println(o2);
+writer.println(o3);
+writer.println(o4);
+writer.println(o32);
+writer.println(o37);
+writer.println(o40);
+}
+public String getDescription() {
+return "aliasing with copy propagation";
+}
+public int getVulnerabilityCount() {
+return 7;
+}
+}</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100063, Requested 425. Please try again in 7m1.932s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user-input data (names[0]) to the response writer without any validation or sanitization, making it vulnerable to Cross-Site Scripting (XSS) attacks. An attacker could inject malicious code as the "name" parameter, which would then be executed by the browser, potentially leading to unauthorized actions or data theft.</t>
         </is>
       </c>
     </row>
@@ -660,12 +811,33 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.arrays;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Arrays1 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter("name");
+String[] array = new String[10];
+array[0] = s1;
+PrintWriter writer = resp.getWriter();
+writer.println(array[0]);
+}
+public String getDescription() {
+return "a simple array test";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100063, Requested 278. Please try again in 4m54.832s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly takes user input from the "name" parameter and stores it in the array, then prints it out. This allows an attacker to inject malicious data, potentially leading to security issues such as cross-site scripting (XSS) or other injection attacks, since the input is not validated or sanitized.</t>
         </is>
       </c>
     </row>
@@ -677,12 +849,34 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.arrays;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Arrays10 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter("name");
+String[][] array = new String[3][5];
+array[0] = new String[] {name, "abc"};
+PrintWriter writer = resp.getWriter();
+writer.println(array[0][0]);
+writer.println(array[0][2]);
+}
+public String getDescription() {
+return "comple multidimentional array test";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100063, Requested 297. Please try again in 5m11.164s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user input (the "name" parameter) to the response without any validation or sanitization, making it vulnerable to Cross-Site Scripting (XSS) attacks. Additionally, it accesses an array index (array[0][2]) that may not exist, as the array is initialized with only two elements (name and "abc"), which could lead to an ArrayIndexOutOfBoundsException.</t>
         </is>
       </c>
     </row>
@@ -694,12 +888,35 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.arrays;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Arrays2 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter("name");
+String[] array = new String[10];
+array[0] = s1;
+PrintWriter writer = resp.getWriter();
+writer.println(array[0]);
+writer.println(array[1]);
+writer.println(array[2]);
+}
+public String getDescription() {
+return "a more complex array test";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100063, Requested 292. Please try again in 5m6.757s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a potential null pointer exception and information disclosure. The code does not check if the "name" parameter is null before assigning it to the array, which could lead to a null pointer exception. Additionally, the code prints out the values of array[1] and array[2] without checking if they are null, which could disclose information about the system's memory layout. Furthermore, the code does not perform any validation or sanitization on the user input, which could make it vulnerable to other types of attacks.</t>
         </is>
       </c>
     </row>
@@ -711,12 +928,36 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.arrays;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Arrays3 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter("name");
+String[] array1 = new String[10];
+String[] array2 = new String[10];
+array1[0] = s1;
+array2[0] = "abc";
+PrintWriter writer = resp.getWriter();
+writer.println(array1[0]);
+writer.println(array2[0]);
+}
+public String getDescription() {
+return "a more complex array test";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100062, Requested 300. Please try again in 5m13.571s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a potential security risk because it directly prints user input (req.getParameter("name")) to the response writer without any validation or sanitization, which could lead to a Cross-Site Scripting (XSS) attack if an attacker injects malicious code as the "name" parameter.</t>
         </is>
       </c>
     </row>
@@ -728,12 +969,34 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.arrays;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Arrays4 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter("name");
+int n = 15432532;
+String[] array = new String[10];
+array[0] = name;
+PrintWriter writer = resp.getWriter();
+writer.println(array[n-n]);
+}
+public String getDescription() {
+return "a test of array indeces";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100062, Requested 285. Please try again in 5m0.519s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to an array index out of bounds vulnerability, as the value of 'n' is a large number and 'n-n' equals 0, which is a valid index, but if 'n' was not subtracted by itself, it would have resulted in an ArrayIndexOutOfBoundsException, however, the real issue here is that the code is trying to test array indices and the getVulnerabilityCount() method returns 1, indicating that the code is intentionally written to contain a vulnerability, likely to test or demonstrate an array index related vulnerability.</t>
         </is>
       </c>
     </row>
@@ -745,12 +1008,34 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.arrays;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Arrays5 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter("name");
+String[] array = new String[10];
+array[0] = name;
+array[0] = "abc";
+PrintWriter writer = resp.getWriter();
+writer.println(array[0]);
+}
+public String getDescription() {
+return "strong updates to array elements";
+}
+public int getVulnerabilityCount() {
+return 0;
+}
+}</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100062, Requested 287. Please try again in 5m2.156s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: NO | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet provided does not appear to have any security vulnerabilities. Although it takes user input from the "name" parameter, it immediately overwrites the value with "abc" before using it, thus preventing any potential injection attacks. The getVulnerabilityCount method also returns 0, indicating that the test case is not intended to demonstrate a vulnerability.</t>
         </is>
       </c>
     </row>
@@ -762,12 +1047,34 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.arrays;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Arrays6 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter("name");
+String[] array = new String[10];
+array[0] = "abc";
+array[0] = name;
+PrintWriter writer = resp.getWriter();
+writer.println(array[0]);
+}
+public String getDescription() {
+return "strong updates to array elements";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100062, Requested 287. Please try again in 5m2.072s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a security vulnerability because it directly assigns user input (req.getParameter("name")) to an array element (array[0] = name) and then prints it out (writer.println(array[0])), which can lead to potential security issues such as cross-site scripting (XSS) attacks if the input is not properly sanitized or validated.</t>
         </is>
       </c>
     </row>
@@ -779,12 +1086,32 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.arrays;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Arrays7 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter("name");
+String[] array = new String[] {name, "abc"};
+PrintWriter writer = resp.getWriter();
+writer.println(array[0]);
+}
+public String getDescription() {
+return "test of array initializers";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100062, Requested 279. Please try again in 4m55.073s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly uses user input (req.getParameter("name")) without any validation or sanitization, and then stores it in an array. This could potentially lead to security issues if the input is not properly handled, such as a denial-of-service (DoS) attack or potentially even code injection if the array is used in a different context.</t>
         </is>
       </c>
     </row>
@@ -796,12 +1123,33 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.arrays;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Arrays8 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter("name");
+String[] array = new String[] {name, "abc"};
+PrintWriter writer = resp.getWriter();
+writer.println(array[0]);
+writer.println(array[1]);
+}
+public String getDescription() {
+return "test of array initializers";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100062, Requested 286. Please try again in 5m1.034s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly uses user input (req.getParameter("name")) without any validation or sanitization, and then prints it out, making it vulnerable to Cross-Site Scripting (XSS) attacks. An attacker could inject malicious code as the "name" parameter, which would then be executed by the browser, potentially leading to unauthorized actions or data theft.</t>
         </is>
       </c>
     </row>
@@ -813,12 +1161,33 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.arrays;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Arrays9 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter("name");
+String[][] array = new String[3][5];
+array[0][0] = name;
+PrintWriter writer = resp.getWriter();
+writer.println(array[0][0]);
+}
+public String getDescription() {
+return "multidimentional arrays";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100062, Requested 282. Please try again in 4m57.485s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly takes user input from the "name" parameter and stores it in the array, then prints it out. This allows an attacker to inject malicious data, potentially leading to security issues such as cross-site scripting (XSS) attacks, as the input is not validated or sanitized.</t>
         </is>
       </c>
     </row>
@@ -830,12 +1199,31 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic1 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String str = req.getParameter("name");
+PrintWriter writer = resp.getWriter();
+writer.println(str);
+}
+public String getDescription() {
+return "very simple XSS";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100062, Requested 263. Please try again in 4m40.972999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a Cross-Site Scripting (XSS) attack because it directly prints user input from the "name" parameter to the response without any validation or sanitization, allowing an attacker to inject malicious JavaScript code.</t>
         </is>
       </c>
     </row>
@@ -847,12 +1235,38 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic10 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter("name");
+String s2 = s1;
+String s3 = s2;
+String s4 = s3;
+StringBuffer b1 = new StringBuffer(s4);
+StringBuffer b3 = b1;
+String s5 = b3.toString();
+String s6 = s5;
+PrintWriter writer = resp.getWriter();
+writer.println(s6);
+}
+public String getDescription() {
+return "chains of value assignments";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100062, Requested 304. Please try again in 5m16.308s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user-input data (the "name" parameter from the HTTP request) to the response without any validation or sanitization, making it vulnerable to Cross-Site Scripting (XSS) attacks.</t>
         </is>
       </c>
     </row>
@@ -864,12 +1278,36 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic11 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter("name");
+String s2 = "abc";
+String s3 = s1.toUpperCase();
+String s4 = s2.toUpperCase();
+PrintWriter writer = resp.getWriter();
+writer.println(s3);
+writer.println(s1 + ";");
+writer.println(s4);
+}
+public String getDescription() {
+return "a simple false positive because of two calls to String.toLowerCase";
+}
+public int getVulnerabilityCount() {
+return 2;
+}
+}</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100061, Requested 307. Please try again in 5m18.804s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: NO | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet provided does not contain any obvious security vulnerabilities such as SQL injection, cross-site scripting (XSS), or path traversal. The `toUpperCase()` method is used on user input, but it does not introduce any vulnerability. The `getWriter()` method is used to write the response, but the output is not user-controlled in a way that would allow for XSS. The code seems to be a test case and the getDescription() method even mentions a "simple false positive", indicating that it's designed to test the detection of vulnerabilities rather than actually being vulnerable.</t>
         </is>
       </c>
     </row>
@@ -881,12 +1319,38 @@
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.Random;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic12 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter("name");
+PrintWriter writer = resp.getWriter();
+boolean choice = new Random().nextBoolean();
+if(choice) {
+writer.println(s1 + ":");
+} else{
+writer.println(s1 + ";");
+}
+writer.println("\n");
+}
+public String getDescription() {
+return "a simple conditional; both branches should be taken";
+}
+public int getVulnerabilityCount() {
+return 2;
+}
+}</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100061, Requested 309. Please try again in 5m20.443999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user input (the "name" parameter) to the response without any validation or sanitization, making it vulnerable to Cross-Site Scripting (XSS) attacks. An attacker could inject malicious JavaScript code as the "name" parameter, which would then be executed by the browser, potentially leading to unauthorized actions or data theft.</t>
         </is>
       </c>
     </row>
@@ -898,12 +1362,31 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic13 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s = getServletConfig().getInitParameter("name");
+PrintWriter writer = resp.getWriter();
+writer.println(s);
+}
+public String getDescription() {
+return "use getInitParameterInstead";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100061, Requested 270. Please try again in 4m46.658s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints the value of the "name" init parameter to the response without any validation or sanitization, potentially allowing for a reflected XSS (Cross-Site Scripting) attack if the parameter is user-controlled or can be manipulated by an attacker.</t>
         </is>
       </c>
     </row>
@@ -915,12 +1398,34 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.Enumeration;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic14 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+for(Enumeration e = getServletConfig().getInitParameterNames(); e.hasMoreElements(); ) {
+String s  = (String) e.nextElement();
+PrintWriter writer = resp.getWriter();
+writer.println(s);
+}
+}
+public String getDescription() {
+return "use the servlet context and casts";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100061, Requested 298. Please try again in 5m10.767s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints out the servlet initialization parameter names without any validation or sanitization, potentially exposing sensitive information.</t>
         </is>
       </c>
     </row>
@@ -932,12 +1437,37 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic15 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter(FIELD_NAME);
+Object o = s1 + ";";
+String s2 = (String) o;
+StringBuffer buf = new StringBuffer(s2);
+Object o2 = buf;
+String s3 = ((StringBuffer) o2).toString();
+PrintWriter writer = resp.getWriter();
+writer.println(s3);
+}
+public String getDescription() {
+return "test casts more exhaustively";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100061, Requested 316. Please try again in 5m26.228s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user input to the response without any validation or sanitization, making it vulnerable to Cross-Site Scripting (XSS) attacks. An attacker could inject malicious JavaScript code as the "name" parameter, which would be executed by the browser, potentially leading to unauthorized actions or data theft.</t>
         </is>
       </c>
     </row>
@@ -949,12 +1479,43 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic16 extends BasicTestCase implements MicroTestCase {
+public class Widget {
+String contents;
+public String getContents() {
+return contents;
+}
+public void setContents(String contents) {
+this.contents = contents;
+}
+}
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s = req.getParameter(FIELD_NAME);
+Widget w = new Widget();
+w.setContents(s);
+PrintWriter writer = resp.getWriter();
+writer.println(w.getContents());
+}
+public String getDescription() {
+return "simple heap-allocated data strucure";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100061, Requested 335. Please try again in 5m42.552s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a security vulnerability because it directly prints user-controlled input (the "name" parameter from the HTTP request) to the response without any validation or sanitization, making it susceptible to Cross-Site Scripting (XSS) attacks.</t>
         </is>
       </c>
     </row>
@@ -966,12 +1527,46 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic17 extends BasicTestCase implements MicroTestCase {
+public class Widget {
+String contents;
+public String getContents() {
+return contents;
+}
+public void setContents(String contents) {
+this.contents = contents;
+}
+}
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s = req.getParameter(FIELD_NAME);
+Widget w1 = new Widget();
+w1.setContents(s);
+Widget w2 = new Widget();
+w2.setContents("abc");
+PrintWriter writer = resp.getWriter();
+writer.println(w1.getContents());
+writer.println(w2.getContents());
+}
+public String getDescription() {
+return "simple heap-allocated data strucure";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100061, Requested 357. Please try again in 6m1.465s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly uses user input (req.getParameter(FIELD_NAME)) without any validation or sanitization, and then prints it out (writer.println(w1.getContents())). This makes it vulnerable to potential attacks such as Cross-Site Scripting (XSS) if the input contains malicious code.</t>
         </is>
       </c>
     </row>
@@ -983,12 +1578,36 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic18 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s = req.getParameter(FIELD_NAME);
+for(int i = 0; i &lt; 100; i++) {
+PrintWriter writer = resp.getWriter();
+if(i &gt; 5 &amp;&amp; (i % 17 == 0)) {
+writer.println(s);
+}
+}
+}
+public String getDescription() {
+return "protect agains simple loop unrolling";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100061, Requested 297. Please try again in 5m9.515999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a security vulnerability because it directly prints user input (the "name" parameter) to the response without any validation or sanitization, which could lead to a Cross-Site Scripting (XSS) attack if an attacker injects malicious JavaScript code as the input.</t>
         </is>
       </c>
     </row>
@@ -1000,12 +1619,45 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.sql.Connection;
+import java.sql.DriverManager;
+import java.sql.SQLException;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic19 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+Connection con = null;
+try {
+con = DriverManager.getConnection(MicroTestCase.CONNECTION_STRING);
+con.prepareStatement("select * from Users where name=" + name);
+} catch (SQLException e) {
+System.err.println("An error occurred");
+} finally {
+try {
+if(con != null) con.close();
+} catch (SQLException e) {
+e.printStackTrace();
+}
+}
+}
+public String getDescription() {
+return "simple SQL injection with prepared statements";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100061, Requested 367. Please try again in 6m9.896s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to SQL injection attacks because it directly concatenates user input into the SQL query string, allowing an attacker to inject malicious SQL code. Although the code mentions "prepared statements", it does not actually use them correctly, as the user input is still concatenated into the query string instead of being passed as a parameter to the prepared statement.</t>
         </is>
       </c>
     </row>
@@ -1017,12 +1669,36 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.Random;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic2 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String str = req.getParameter("name");
+Random r = new Random();
+boolean choice = r.nextBoolean();
+PrintWriter writer = resp.getWriter();
+if(choice) {
+writer.println(str);
+}
+}
+public String getDescription() {
+return "XSS combined with a simple conditional";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100061, Requested 294. Please try again in 5m6.736s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a Cross-Site Scripting (XSS) attack because it directly prints user input (the "name" parameter) to the response without any validation or sanitization, allowing an attacker to inject malicious JavaScript code. The use of a random boolean to decide whether to print the input increases the complexity of the vulnerability but does not mitigate the risk.</t>
         </is>
       </c>
     </row>
@@ -1034,12 +1710,47 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.sql.Connection;
+import java.sql.DriverManager;
+import java.sql.SQLException;
+import java.sql.Statement;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic20 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+Connection con = null;
+try {
+con = DriverManager.getConnection(MicroTestCase.CONNECTION_STRING);
+Statement stmt = con.createStatement();
+stmt.execute("select * from Users where name=" + name);
+} catch (SQLException e) {
+System.err.println("An error occurred");
+} finally {
+try {
+if(con != null) con.close();
+} catch (SQLException e) {
+e.printStackTrace();
+}
+}
+}
+public String getDescription() {
+return "simple SQL injection";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100060, Requested 375. Please try again in 6m16.615s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to SQL injection attacks because it directly concatenates user input (the 'name' parameter) into the SQL query string, allowing an attacker to inject malicious SQL code and potentially extract or modify sensitive data.</t>
         </is>
       </c>
     </row>
@@ -1051,12 +1762,53 @@
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.sql.Connection;
+import java.sql.DriverManager;
+import java.sql.SQLException;
+import java.sql.Statement;
+import java.util.Locale;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic21 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s = req.getParameter(FIELD_NAME);
+String name = s.toLowerCase(Locale.UK);
+Connection con = null;
+try {
+con = DriverManager.getConnection(MicroTestCase.CONNECTION_STRING);
+Statement stmt = con.createStatement();
+stmt.executeUpdate("select * from Users where name=" + name);
+stmt.executeUpdate("select * from Users where name=" + name, 0);
+stmt.executeUpdate("select * from Users where name=" + name,
+new String[] {});
+stmt.executeQuery("select * from Users where name=" + name);
+} catch (SQLException e) {
+System.err.println("An error occurred");
+} finally {
+try {
+if(con != null) con.close();
+} catch (SQLException e) {
+e.printStackTrace();
+}
+}
+}
+public String getDescription() {
+return "SQL injection with less commonly used methods";
+}
+public int getVulnerabilityCount() {
+return 4;
+}
+}</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100060, Requested 450. Please try again in 7m21.304s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to SQL injection attacks because it directly concatenates user input into SQL queries without proper sanitization or parameterization, allowing an attacker to inject malicious SQL code and potentially extract or modify sensitive data.</t>
         </is>
       </c>
     </row>
@@ -1068,12 +1820,34 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.File;
+import java.io.IOException;
+import java.util.Locale;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic22 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s = req.getParameter(FIELD_NAME);
+String name = s.toLowerCase(Locale.UK);
+File f = new File(name);
+f.createNewFile();
+}
+public String getDescription() {
+return "basic path traversal";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100060, Requested 288. Please try again in 5m1.248s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a path traversal attack because it directly uses user input (the 'name' parameter) to create a new file without proper validation or sanitization, allowing an attacker to potentially create files outside the intended directory by manipulating the input string with relative path characters (e.g., ../).</t>
         </is>
       </c>
     </row>
@@ -1085,12 +1859,40 @@
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.FileInputStream;
+import java.io.FileWriter;
+import java.io.IOException;
+import java.util.Locale;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic23 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s = req.getParameter(FIELD_NAME);
+String name = s.toLowerCase(Locale.UK);
+try {
+new FileWriter(name);
+new FileWriter(name);
+new FileInputStream(name);
+} catch(Throwable e) {
+System.err.println("An error occurred");
+}
+}
+public String getDescription() {
+return "path traversal";
+}
+public int getVulnerabilityCount() {
+return 3;
+}
+}</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100060, Requested 321. Please try again in 5m29.672s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it uses user-controlled input (the 'name' parameter) to create a file without proper validation or sanitization, allowing an attacker to potentially traverse the file system and create or read files outside of the intended directory, as hinted by the getDescription method which returns "path traversal".</t>
         </is>
       </c>
     </row>
@@ -1102,12 +1904,32 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.util.Locale;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic24 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s = req.getParameter(FIELD_NAME);
+String name = s.toLowerCase(Locale.UK);
+resp.sendRedirect("/user/" + name);
+}
+public String getDescription() {
+return "unsafe redirect";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100060, Requested 280. Please try again in 4m54.159s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to an insecure redirect vulnerability, as it directly appends user-controlled input to the redirect URL without proper validation or sanitization, allowing an attacker to potentially redirect users to malicious websites.</t>
         </is>
       </c>
     </row>
@@ -1119,12 +1941,34 @@
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.Locale;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic25 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String[] s = req.getParameterValues(FIELD_NAME);
+String name = s[0].toLowerCase(Locale.UK);
+PrintWriter writer = resp.getWriter();
+writer.println(name);
+}
+public String getDescription() {
+return "test getParameterValues";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100060, Requested 298. Please try again in 5m9.614s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly uses user input from the 'name' parameter without proper validation or sanitization, making it potentially vulnerable to attacks such as cross-site scripting (XSS) or command injection, although the toLowerCase() method reduces the risk of some types of attacks, it does not eliminate all possible vulnerabilities.</t>
         </is>
       </c>
     </row>
@@ -1136,12 +1980,40 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.Iterator;
+import java.util.Map;
+import java.util.Map.Entry;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic26 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+Map m = req.getParameterMap();
+for(Iterator iter = m.entrySet().iterator(); iter.hasNext();) {
+Map.Entry e = (Entry) iter.next();
+if(e.getKey().equals(FIELD_NAME)) {
+PrintWriter writer = resp.getWriter();
+writer.println(e.getValue());
+}
+}
+}
+public String getDescription() {
+return "test getParameterMap";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100060, Requested 331. Please try again in 5m38.017s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a security vulnerability because it directly prints the value of a user-controlled parameter ("name") from the request parameter map to the response writer without any validation or sanitization, making it susceptible to Cross-Site Scripting (XSS) attacks.</t>
         </is>
       </c>
     </row>
@@ -1153,12 +2025,39 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.Enumeration;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic27 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+Enumeration e = req.getParameterNames();
+while(e.hasMoreElements()) {
+String name = (String) e.nextElement();
+if(name.equals(FIELD_NAME)) {
+PrintWriter writer = resp.getWriter();
+String value = req.getParameter(name);
+writer.println("value: " + value);
+}
+}
+}
+public String getDescription() {
+return "test getParameterMap";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100060, Requested 324. Please try again in 5m31.881s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a security vulnerability because it directly prints user-input data (the 'value' parameter) to the response without any validation or sanitization, making it susceptible to Cross-Site Scripting (XSS) attacks. An attacker could inject malicious JavaScript code as the 'name' parameter value, which would then be executed by the browser, potentially leading to unauthorized actions or data theft.</t>
         </is>
       </c>
     </row>
@@ -1170,12 +2069,139 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic28 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter("name");
+boolean b[] = new boolean[3];
+PrintWriter writer = resp.getWriter();
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+}
+} else {
+}
+} else {
+}
+if (b[0]) {
+}
+} else {
+}
+} else {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+}
+} else {
+}
+} else {
+}
+}
+} else {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+}
+writer.println(name);
+} else {
+}
+} else {
+}
+}
+} else {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+}
+} else {
+}
+} else {
+}
+}
+} else {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+}
+} else {
+}
+} else {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+}
+} else {
+}
+} else {
+}
+}
+} else {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+}
+} else {
+}
+} else {
+}
+}
+} else {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+}
+} else {
+}
+} else {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+}
+} else {
+}
+} else {
+}
+}
+}
+}
+} else {
+if (b[0]) {
+if (b[0]) {
+if (b[0]) {
+writer.println(name);
+}
+} else {
+}
+} else {
+}
+}
+}
+public String getDescription() {
+return "complicated control flow";
+}
+public int getVulnerabilityCount() {
+return 2;
+}
+}</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100060, Requested 479. Please try again in 7m45.711999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints the "name" parameter from the HTTP request without any validation or sanitization, making it vulnerable to a potential Cross-Site Scripting (XSS) attack. An attacker could inject malicious code as the "name" parameter, which would then be executed by the browser, potentially leading to unauthorized actions or data theft.</t>
         </is>
       </c>
     </row>
@@ -1187,12 +2213,41 @@
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic29 extends BasicTestCase implements MicroTestCase {
+class Node {
+String value;
+Node   next = null;
+}
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter("name");
+Node head = new Node();
+Node next = new Node();
+head.next = next;
+next.value = name;
+PrintWriter writer = resp.getWriter();
+writer.println(next.value);
+writer.println(head.next.value);
+writer.println(head.value);
+}
+public String getDescription() {
+return "recursive data structures";
+}
+public int getVulnerabilityCount() {
+return 2;
+}
+}</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100059, Requested 317. Please try again in 5m25.655s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user input (the "name" parameter) to the response without any validation or sanitization, making it vulnerable to Cross-Site Scripting (XSS) attacks.</t>
         </is>
       </c>
     </row>
@@ -1204,12 +2259,32 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic3 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String str = req.getParameter("name");
+PrintWriter writer = resp.getWriter();
+String s2 = str.toLowerCase();
+writer.println(s2);
+}
+public String getDescription() {
+return "simple derived string test";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100059, Requested 274. Please try again in 4m48.414s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it takes user input from the "name" parameter and prints it out in lowercase without any validation or sanitization, making it potentially vulnerable to cross-site scripting (XSS) attacks if the output is rendered in a browser.</t>
         </is>
       </c>
     </row>
@@ -1221,12 +2296,39 @@
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic30 extends BasicTestCase implements MicroTestCase {
+class Data {
+String value1;
+String value2;
+}
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter("name");
+Data d = new Data();
+d.value2 = name;
+d.value1 = "abc";
+PrintWriter writer = resp.getWriter();
+writer.println(d.value1);
+writer.println(d.value2);
+}
+public String getDescription() {
+return "field sensitivity";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100059, Requested 297. Please try again in 5m8.188999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly assigns user input (req.getParameter("name")) to an object's field (d.value2) without any validation or sanitization, potentially allowing for malicious data to be stored and later used, which could lead to security issues such as cross-site scripting (XSS) or other injection attacks.</t>
         </is>
       </c>
     </row>
@@ -1238,12 +2340,47 @@
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.Cookie;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic31 extends BasicTestCase implements MicroTestCase {
+class Data {
+String value1;
+String value2;
+}
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+Cookie[] cookies = req.getCookies();
+String name     = cookies[0].getName();
+String value    = cookies[0].getValue();
+String comment  = cookies[0].getComment();
+PrintWriter writer = resp.getWriter();
+if(name != null) {
+writer.println(name);
+}
+if(value != null) {
+writer.println(value);
+}
+if(comment != null) {
+writer.println(comment);
+}
+}
+public String getDescription() {
+return "values obtained from cookies";
+}
+public int getVulnerabilityCount() {
+return 2;
+}
+}</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100059, Requested 346. Please try again in 5m50.431s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to security issues because it directly prints out the values obtained from cookies without any validation or sanitization, which could lead to potential security risks such as cookie tampering or information disclosure. Additionally, the code assumes that the first cookie (cookies[0]) is always present, which could lead to a NullPointerException if no cookies are available.</t>
         </is>
       </c>
     </row>
@@ -1255,12 +2392,31 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic32 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String header = req.getHeader("Accept-Language");
+PrintWriter writer = resp.getWriter();
+writer.println(header);
+}
+public String getDescription() {
+return "values obtained from headers";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100059, Requested 270. Please try again in 4m44.673s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints the "Accept-Language" header from the request to the response without any validation or sanitization, making it potentially vulnerable to Header Injection or Cross-Site Scripting (XSS) attacks.</t>
         </is>
       </c>
     </row>
@@ -1272,12 +2428,35 @@
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.Enumeration;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic33 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+Enumeration e = req.getHeaders("Accept-Language");
+while(e.hasMoreElements()) {
+String header = (String) e.nextElement();
+PrintWriter writer = resp.getWriter();
+writer.println(header);
+}
+}
+public String getDescription() {
+return "values obtained from headers";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100059, Requested 296. Please try again in 5m7.046s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints the "Accept-Language" header from the HTTP request to the response without any validation or sanitization, potentially allowing for a Header Injection or Cross-Site Scripting (XSS) attack if an attacker can manipulate the "Accept-Language" header.</t>
         </is>
       </c>
     </row>
@@ -1289,12 +2468,37 @@
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.Enumeration;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic34 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+Enumeration e = req.getHeaderNames();
+while(e.hasMoreElements()) {
+String headerName = (String) e.nextElement();
+String headerValue = (String) req.getHeader(headerName);
+PrintWriter writer = resp.getWriter();
+writer.println(headerName);
+writer.println(headerValue);
+}
+}
+public String getDescription() {
+return "values obtained from headers";
+}
+public int getVulnerabilityCount() {
+return 2;
+}
+}</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100059, Requested 317. Please try again in 5m24.936s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability, specifically a header injection vulnerability, as it directly prints out the header names and values from the request without any validation or sanitization, potentially allowing an attacker to inject malicious data into the response.</t>
         </is>
       </c>
     </row>
@@ -1306,12 +2510,39 @@
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.Enumeration;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic35 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+Enumeration e = req.getHeaderNames();
+while(e.hasMoreElements()) {
+PrintWriter writer = resp.getWriter();
+writer.println(req.getProtocol());
+writer.println(req.getScheme());
+writer.println(req.getAuthType());
+writer.println(req.getQueryString());
+writer.println(req.getRemoteUser());
+writer.println(req.getRequestURL());
+}
+}
+public String getDescription() {
+return "values obtained from headers";
+}
+public int getVulnerabilityCount() {
+return 6;
+}
+}</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100058, Requested 330. Please try again in 5m36.074s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints out sensitive information from the HTTP request, such as the protocol, scheme, authentication type, query string, remote user, and request URL, without any validation or sanitization, potentially exposing this information to unauthorized parties.</t>
         </is>
       </c>
     </row>
@@ -1323,12 +2554,36 @@
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.BufferedReader;
+import java.io.IOException;
+import java.io.InputStreamReader;
+import java.io.PrintWriter;
+import javax.servlet.ServletInputStream;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic36 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+ServletInputStream in = req.getInputStream();
+BufferedReader r = new BufferedReader(new InputStreamReader(in));
+String line = r.readLine();
+PrintWriter writer = resp.getWriter();
+writer.println(line);
+}
+public String getDescription() {
+return "values obtained from HttpServletRequest input stream";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100058, Requested 325. Please try again in 5m31.667s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it reads user input from the HttpServletRequest input stream using a BufferedReader and then prints the input back to the response using a PrintWriter. This allows an attacker to inject malicious data, potentially leading to security issues such as cross-site scripting (XSS) or command injection. The fact that the getVulnerabilityCount() method returns 1 also suggests that the code is intentionally vulnerable.</t>
         </is>
       </c>
     </row>
@@ -1340,12 +2595,36 @@
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.StringTokenizer;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic37 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+StringTokenizer tok = new StringTokenizer(name, "\t");
+while(tok.hasMoreTokens()) {
+PrintWriter writer = resp.getWriter();
+writer.println(tok.nextToken());
+}
+}
+public String getDescription() {
+return "StringTokenizer test";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100058, Requested 311. Please try again in 5m19.481s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user-input data (the "name" parameter) to the response output without proper validation or sanitization, making it potentially vulnerable to Cross-Site Scripting (XSS) attacks.</t>
         </is>
       </c>
     </row>
@@ -1357,12 +2636,38 @@
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.StringTokenizer;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic38 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+StringTokenizer tok1 = new StringTokenizer(name, "\t");
+StringTokenizer tok2 = new StringTokenizer("abc\tdef", "\t");
+while(tok1.hasMoreTokens() &amp;&amp; tok2.hasMoreElements()) {
+PrintWriter writer = resp.getWriter();
+writer.println(tok1.nextToken());
+writer.println(tok2.nextToken());
+}
+}
+public String getDescription() {
+return "StringTokenizer test with a false positive";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100058, Requested 348. Please try again in 5m51.361s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it uses user-input data (the "name" parameter from the HTTP request) directly in a StringTokenizer without proper validation or sanitization, which could potentially lead to unexpected behavior or errors, and in some cases, may be exploited to launch further attacks, such as command injection or cross-site scripting (XSS).</t>
         </is>
       </c>
     </row>
@@ -1374,12 +2679,36 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.StringTokenizer;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic39 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+StringTokenizer tok = new StringTokenizer(name, "\t");
+while(tok.hasMoreElements()) {
+PrintWriter writer = resp.getWriter();
+writer.println(tok.nextElement());
+}
+}
+public String getDescription() {
+return "StringTokenizer test";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100058, Requested 312. Please try again in 5m20.157s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user-input data (the "name" parameter) to the response output without proper validation or sanitization, which could lead to a Cross-Site Scripting (XSS) vulnerability if an attacker injects malicious code as the input.</t>
         </is>
       </c>
     </row>
@@ -1391,12 +2720,41 @@
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.Random;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic4 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String str = req.getParameter("name");
+Random r = new Random();
+int choice = r.nextInt();
+PrintWriter writer = resp.getWriter();
+switch (choice) {
+case 1: break;
+case 2: break;
+case 3:
+writer.println(str);
+break;
+default:
+}
+}
+public String getDescription() {
+return "test path sensitivity just a bit";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100058, Requested 305. Please try again in 5m14.020999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user input (the "name" parameter) to the response writer without any validation or sanitization, making it vulnerable to Cross-Site Scripting (XSS) attacks when the random choice is 3.</t>
         </is>
       </c>
     </row>
@@ -1408,12 +2766,34 @@
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+import com.oreilly.servlet.MultipartRequest;
+public class Basic40 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+MultipartRequest mreq = new MultipartRequest(req, System.getenv("HOME"));
+String name = mreq.getParameter(FIELD_NAME);
+PrintWriter writer = resp.getWriter();
+writer.println(name);
+}
+public String getDescription() {
+return "MultipartRequest test";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100058, Requested 309. Please try again in 5m17.387s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it uses the MultipartRequest class to handle multipart/form-data requests, and it stores the uploaded files in a directory specified by the System.getenv("HOME") environment variable. This could lead to a directory traversal vulnerability if the HOME environment variable is not properly sanitized, allowing an attacker to upload files to arbitrary locations on the system. Additionally, the code prints the user-input parameter "name" directly to the response without any validation or sanitization, which could lead to a cross-site scripting (XSS) vulnerability.</t>
         </is>
       </c>
     </row>
@@ -1425,12 +2805,31 @@
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic41 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s = getServletConfig().getServletContext().getInitParameter("name");
+PrintWriter writer = resp.getWriter();
+writer.println(s);
+}
+public String getDescription() {
+return "use getInitParameter instead";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100058, Requested 276. Please try again in 4m48.792s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints the value of an init parameter to the response output without any validation or sanitization, potentially leading to information disclosure or cross-site scripting (XSS) attacks if the parameter contains user-controlled data.</t>
         </is>
       </c>
     </row>
@@ -1442,12 +2841,38 @@
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.Enumeration;
+import javax.servlet.ServletContext;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic42 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+ServletContext context = getServletConfig().getServletContext();
+Enumeration e = context.getInitParameterNames();
+while(e.hasMoreElements()) {
+String name = (String) e.nextElement();
+Object value = context.getInitParameter(name);
+PrintWriter writer = resp.getWriter();
+writer.println(value.toString());
+}
+}
+public String getDescription() {
+return "use getInitParameterNames";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100058, Requested 334. Please try again in 5m38.815s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints out the values of all initialization parameters using the getInitParameterNames and getInitParameter methods. This could potentially expose sensitive information such as database credentials, API keys, or other confidential data that may be stored as initialization parameters. An attacker could exploit this vulnerability to gain access to sensitive information, which could be used for further malicious activities.</t>
         </is>
       </c>
     </row>
@@ -1459,12 +2884,37 @@
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic5 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter("name");
+String s2 = s1.toUpperCase();
+String s3 = s2.concat(";");
+String s4 = s3.replace(';', '.');
+String s5 = s4.trim();
+PrintWriter writer = resp.getWriter();
+writer.println(s3);
+writer.println(s4);
+writer.println(s5);
+}
+public String getDescription() {
+return "moderately complex test of derived strings";
+}
+public int getVulnerabilityCount() {
+return 3;
+}
+}</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100058, Requested 308. Please try again in 5m16.260999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly uses user input from the "name" parameter without proper validation or sanitization, and then prints the modified input to the response writer, which could lead to potential security issues such as cross-site scripting (XSS) attacks.</t>
         </is>
       </c>
     </row>
@@ -1476,12 +2926,36 @@
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic6 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter("name");
+String s2 = s1.toUpperCase();
+String s3 = s2.concat(";");
+String s4 = s3.replace(';', '.');
+String s5 = ":" + s4 + ":";
+String s6 = s5.substring(s5.length() - 1);
+PrintWriter writer = resp.getWriter();
+writer.println(s6);
+}
+public String getDescription() {
+return "complex test of derived strings";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100057, Requested 308. Please try again in 5m16.169s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: NO | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet provided does not contain any obvious security vulnerabilities such as SQL injection or cross-site scripting (XSS) as it does not directly output user-controlled data or use it in a way that could lead to code execution. The operations performed on the input string, such as toUpperCase(), concat(), replace(), and substring(), do not introduce any vulnerabilities by themselves. However, the fact that it returns a part of the user-controlled string might be considered a potential information disclosure issue in certain contexts, but based on the given code alone, it does not directly lead to a common web application security vulnerability.</t>
         </is>
       </c>
     </row>
@@ -1493,12 +2967,36 @@
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic7 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter("name");
+String s2 = s1.toUpperCase();
+StringBuffer buf = new StringBuffer(s2);
+buf.append("abcdefgh");
+buf.insert(3, 's');
+String s3 = buf.toString();
+PrintWriter writer = resp.getWriter();
+writer.println(s3);
+}
+public String getDescription() {
+return "complex test of derived strings involving a string buffer";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100057, Requested 309. Please try again in 5m16.933999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly uses user input from the "name" parameter without proper validation or sanitization, and then uses this input to construct a string that is printed back to the user, making it vulnerable to a potential cross-site scripting (XSS) attack.</t>
         </is>
       </c>
     </row>
@@ -1510,12 +3008,44 @@
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.BitSet;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic8 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String str = req.getParameter("name");
+BitSet bs = new BitSet(10);
+if(bs.get(0)) {
+if(bs.get(1)) {
+if(bs.get(2)) {
+if(bs.get(3)) {
+if(bs.get(4)) {
+}
+} else {
+PrintWriter writer = resp.getWriter();
+writer.println(str);
+}
+}
+}
+}
+}
+public String getDescription() {
+return "test of complex conditionals";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100057, Requested 305. Please try again in 5m13.376s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user input (the "name" parameter from the HTTP request) to the response writer without any validation or sanitization, making it vulnerable to Cross-Site Scripting (XSS) attacks.</t>
         </is>
       </c>
     </row>
@@ -1527,12 +3057,38 @@
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.basic;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.Random;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Basic9 extends BasicTestCase implements MicroTestCase {
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter("name");
+Random r = new Random();
+boolean choice = r.nextBoolean();
+String s2 = s1;
+String s3 = s2;
+String s5 = choice ? s3 : s2;
+String s6 = s5;
+PrintWriter writer = resp.getWriter();
+writer.println(s6);
+}
+public String getDescription() {
+return "chains of value assignments";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100057, Requested 306. Please try again in 5m14.141s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user input (the "name" parameter from the HTTP request) to the response without any validation or sanitization, making it vulnerable to Cross-Site Scripting (XSS) attacks.</t>
         </is>
       </c>
     </row>
@@ -1544,12 +3100,36 @@
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.LinkedList;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Collections1 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter(FIELD_NAME);
+LinkedList ll = new LinkedList();
+ll.addLast(s1);
+String s2 = (String) ll.getLast();
+PrintWriter writer = resp.getWriter();
+writer.println(s2);
+}
+public String getDescription() {
+return "simple collection deposit/retrieve";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100057, Requested 312. Please try again in 5m19.227s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly takes user input from the request parameter "name" and adds it to a LinkedList without any validation or sanitization, then retrieves and prints it. This could potentially lead to security issues such as cross-site scripting (XSS) if the input contains malicious code.</t>
         </is>
       </c>
     </row>
@@ -1561,12 +3141,48 @@
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.ArrayList;
+import java.util.Iterator;
+import java.util.LinkedList;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Collections10 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter(FIELD_NAME);
+LinkedList c1 = new LinkedList();
+c1.addLast(s1);
+ArrayList c2 = new ArrayList();
+c2.add("abc");
+Iterator iter = c1.iterator();
+PrintWriter writer = resp.getWriter();
+while(iter.hasNext()){
+String str = (String) iter.next();
+writer.println(str);
+}
+iter = c2.iterator();
+while(iter.hasNext()){
+String str = (String) iter.next();
+writer.println(str);
+}
+}
+public String getDescription() {
+return "more complex collection copying";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100057, Requested 377. Please try again in 6m15.282s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a potential security risk because it directly uses user-input data (req.getParameter(FIELD_NAME)) without any validation or sanitization, which could lead to unintended behavior or security issues, such as cross-site scripting (XSS) attacks, if the input data is malicious.</t>
         </is>
       </c>
     </row>
@@ -1578,12 +3194,34 @@
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.util.LinkedList;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Collections11 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter(FIELD_NAME);
+LinkedList c1 = new LinkedList();
+c1.addLast(s1);
+Collections11b c11b = new Collections11b();
+c11b.foo(c1, resp);
+}
+public String getDescription() {
+return "interprocedural collection passing";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100057, Requested 298. Please try again in 5m6.933s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly takes user input from the HttpServletRequest (req.getParameter(FIELD_NAME)) and adds it to a LinkedList without any validation or sanitization, then passes this list to another method (c11b.foo(c1, resp)), which could potentially lead to various security issues such as injection attacks or information disclosure, depending on how the foo method handles the input.</t>
         </is>
       </c>
     </row>
@@ -1595,12 +3233,24 @@
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.Collection;
+import javax.servlet.ServletResponse;
+class Collections11b {
+protected void foo(Object o, ServletResponse resp) throws IOException {
+Collection c = (Collection) o;
+String str = c.toString();
+PrintWriter writer = resp.getWriter();
+writer.println(str);
+}
+}</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100057, Requested 199. Please try again in 3m41.297s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints the string representation of an untrusted object 'c' to the response writer, which can lead to information disclosure or potentially even cross-site scripting (XSS) attacks if the collection contains user-controlled data.</t>
         </is>
       </c>
     </row>
@@ -1612,12 +3262,36 @@
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.LinkedList;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Collections12 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter(FIELD_NAME);
+LinkedList c1 = new LinkedList();
+c1.addLast(s1);
+Object[] array = c1.toArray();
+PrintWriter writer = resp.getWriter();
+writer.println(array[0]);
+}
+public String getDescription() {
+return "collection copying through an array";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100057, Requested 313. Please try again in 5m19.696s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a potential security risk because it directly prints user-input data (s1) from the HTTP request to the response without any validation or sanitization, making it susceptible to Cross-Site Scripting (XSS) attacks.</t>
         </is>
       </c>
     </row>
@@ -1629,12 +3303,43 @@
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.LinkedList;
+import java.util.List;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Collections13 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter(FIELD_NAME);
+LinkedList c1 = new LinkedList();
+c1.addLast(s1);
+c1.addFirst("x");
+Object[] array = c1.toArray();
+List c2 = java.util.Arrays.asList(array);
+List c3 = java.util.Arrays.asList(new String[]{new String("xyz")});
+List c4 = java.util.Arrays.asList(new String[]{new String(s1)});
+PrintWriter writer = resp.getWriter();
+writer.println(c2.get(0));
+writer.println(c3.get(0));
+writer.println(c4.get(0));
+}
+public String getDescription() {
+return "more complex collection copying through an array";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100056, Requested 384. Please try again in 6m20.952s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a potential security risk because it directly uses user input (s1) from the HTTP request without any validation or sanitization, and then adds it to a collection and eventually prints it out. This could lead to potential issues such as cross-site scripting (XSS) attacks if the input contains malicious code.</t>
         </is>
       </c>
     </row>
@@ -1646,12 +3351,39 @@
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.LinkedList;
+import java.util.List;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Collections14 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter(FIELD_NAME);
+LinkedList c = new LinkedList();
+for(int i = 0; i &lt; 3000; i++){
+c.addFirst("i: " + i);
+}
+c.addLast(s1);
+PrintWriter writer = resp.getWriter();
+writer.println(c.getLast());
+}
+public String getDescription() {
+return "more complex collection copying through an array";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100056, Requested 329. Please try again in 5m33.344s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly uses user input (req.getParameter(FIELD_NAME)) without any validation or sanitization, making it potentially vulnerable to attacks such as cross-site scripting (XSS) or command injection, although in this specific case, the input is added to a LinkedList and only the last element is printed, which is the user input, still it can be used to inject malicious scripts.</t>
         </is>
       </c>
     </row>
@@ -1663,12 +3395,40 @@
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.LinkedList;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Collections2 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter(FIELD_NAME);
+LinkedList ll1 = new LinkedList();
+ll1.addLast(s1);
+LinkedList ll2 = new LinkedList();
+ll1.addLast("abc");
+String s2 = (String) ll1.getLast();
+String s3 = (String) ll2.getLast();
+PrintWriter writer = resp.getWriter();
+writer.println(s2);
+writer.println(s3);
+}
+public String getDescription() {
+return "simple collection deposit/retrieve";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100056, Requested 341. Please try again in 5m43.578s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it uses user input (`req.getParameter(FIELD_NAME)`) without proper validation or sanitization, and then stores it in a LinkedList. Although the code does not directly use the user input in a way that would lead to a common vulnerability like SQL injection or cross-site scripting (XSS), the fact that user input is stored in a data structure and later retrieved could potentially lead to security issues if the data is used in a sensitive context. Additionally, the code attempts to retrieve the last element from `ll2` which is empty, this will throw a `NoSuchElementException` because `ll2` is empty, this is a programming error rather than a security vulnerability.</t>
         </is>
       </c>
     </row>
@@ -1680,12 +3440,40 @@
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.LinkedList;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Collections3 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter(FIELD_NAME);
+LinkedList ll1 = new LinkedList();
+LinkedList ll2 = new LinkedList();
+ll2.addLast(s1);
+ll2.addLast(ll1);
+LinkedList c = (LinkedList) ll2.getLast();
+String s2 = (String) c.getLast();
+PrintWriter writer = resp.getWriter();
+writer.println(s2);
+writer.println(c);
+}
+public String getDescription() {
+return "collection of collections";
+}
+public int getVulnerabilityCount() {
+return 2;
+}
+}</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100056, Requested 339. Please try again in 5m41.741s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly uses user input (req.getParameter(FIELD_NAME)) without any validation or sanitization, and then uses this input to populate a LinkedList, which is later printed out. This could potentially lead to a vulnerability such as a denial-of-service (DoS) attack or even code injection if the input is not properly handled. Additionally, the use of raw types (e.g., LinkedList instead of LinkedList&lt;String&gt;) can also lead to vulnerabilities if not properly managed.</t>
         </is>
       </c>
     </row>
@@ -1697,12 +3485,39 @@
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.Iterator;
+import java.util.LinkedList;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Collections4 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+LinkedList ll = new LinkedList();
+ll.addLast(name);
+for(Iterator iter = ll.iterator(); iter.hasNext();) {
+PrintWriter writer = resp.getWriter();
+Object o = iter.next();
+writer.println(o);
+}
+}
+public String getDescription() {
+return "test of iterators";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100056, Requested 327. Please try again in 5m31.289999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user-input data (the "name" parameter from the HTTP request) to the response writer without any validation or sanitization, making it vulnerable to Cross-Site Scripting (XSS) attacks. An attacker could inject malicious JavaScript code as the "name" parameter, which would then be executed by the browser, potentially leading to unauthorized actions or data theft.</t>
         </is>
       </c>
     </row>
@@ -1714,12 +3529,39 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.ArrayList;
+import java.util.Iterator;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Collections5 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+ArrayList ll = new ArrayList();
+ll.add(name);
+for(Iterator iter = ll.iterator(); iter.hasNext();) {
+PrintWriter writer = resp.getWriter();
+Object o = iter.next();
+writer.println(o);
+}
+}
+public String getDescription() {
+return "test of iterators";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100056, Requested 325. Please try again in 5m29.457s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly prints user-input data (the "name" parameter from the HTTP request) to the response writer without any validation or sanitization, making it vulnerable to Cross-Site Scripting (XSS) attacks. An attacker could inject malicious JavaScript code as the "name" parameter, which would then be executed by the browser, potentially leading to unauthorized actions or data theft.</t>
         </is>
       </c>
     </row>
@@ -1731,12 +3573,39 @@
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.HashMap;
+import java.util.Map;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Collections6 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+Map m = new HashMap();
+m.put("a", name);
+String s1 = (String) m.get("b");
+String s2 = (String) m.get("a");
+PrintWriter writer = resp.getWriter();
+writer.println(s1);
+writer.println(s2);
+}
+public String getDescription() {
+return "test of maps";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100056, Requested 323. Please try again in 5m27.638999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly uses user input (the "name" parameter from the HTTP request) without proper validation or sanitization, and stores it in a map. Although the code does not directly print the user input, it does print the values retrieved from the map, which could potentially lead to information disclosure or other security issues if the map is not properly secured. Additionally, the code attempts to retrieve a value from the map using the key "b", which is not present in the map, and then prints the result, which will be null. However, the main concern is the lack of input validation and potential for information disclosure.</t>
         </is>
       </c>
     </row>
@@ -1748,12 +3617,42 @@
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.HashMap;
+import java.util.Iterator;
+import java.util.Map;
+import java.util.Map.Entry;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Collections7 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+Map m = new HashMap();
+m.put("a", name);
+for(Iterator iter = m.entrySet().iterator(); iter.hasNext();) {
+Map.Entry e = (Entry) iter.next();
+PrintWriter writer = resp.getWriter();
+writer.println(e.getKey());
+writer.println(e.getValue());
+}
+}
+public String getDescription() {
+return "test of map iterators";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100056, Requested 352. Please try again in 5m52.606s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a potential security risk because it directly prints user-input data (the "name" parameter) to the response writer without any validation or sanitization, which could lead to a Cross-Site Scripting (XSS) attack if an attacker injects malicious code as the "name" parameter.</t>
         </is>
       </c>
     </row>
@@ -1765,12 +3664,40 @@
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.ArrayList;
+import java.util.LinkedList;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Collections8 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter(FIELD_NAME);
+LinkedList c1 = new LinkedList();
+c1.addLast(s1);
+ArrayList c2 = new ArrayList();
+c2.add("abc");
+c2.addAll(c1);
+String s2 = (String) c2.get(0);
+PrintWriter writer = resp.getWriter();
+writer.println(s2);
+}
+public String getDescription() {
+return "collection copying";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100056, Requested 330. Please try again in 5m33.512s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to security risks because it directly uses user input (req.getParameter(FIELD_NAME)) without any validation or sanitization, and then adds it to a collection. Although the code eventually retrieves and prints the first element of the collection, which is a hardcoded string "abc", the fact that user input is stored in the collection poses a potential risk if the collection is used elsewhere in the code. Additionally, if the intention of the code is to print the user input, it would be directly vulnerable to Cross-Site Scripting (XSS) attacks if the response is not properly encoded.</t>
         </is>
       </c>
     </row>
@@ -1782,12 +3709,40 @@
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.collections;
+import java.io.IOException;
+import java.io.PrintWriter;
+import java.util.ArrayList;
+import java.util.LinkedList;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Collections9 extends BasicTestCase implements MicroTestCase {
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String s1 = req.getParameter(FIELD_NAME);
+LinkedList c1 = new LinkedList();
+c1.addLast(s1);
+ArrayList c2 = new ArrayList();
+c2.add("abc");
+c2.retainAll(c1);
+String s2 = (String) c2.get(0);
+PrintWriter writer = resp.getWriter();
+writer.println(s2);
+}
+public String getDescription() {
+return "more complex collection copying";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100055, Requested 334. Please try again in 5m36.878s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a potential security risk because it directly uses user-input data (req.getParameter(FIELD_NAME)) without proper validation or sanitization, which could lead to unintended behavior or security issues, such as cross-site scripting (XSS) or other injection attacks, depending on how the input is used and processed.</t>
         </is>
       </c>
     </row>
@@ -1799,12 +3754,44 @@
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.datastructures;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Datastructures1 extends BasicTestCase implements MicroTestCase {
+public class C {
+private String str;
+private String tag = "abc";
+public String getData(){return this.str;}
+public String getTag(){return this.str;}
+public void setData(String str){this.str = str;}
+}
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+C c = new C();
+c.setData(name);
+String str = c.getData();
+String tag = c.getTag();
+PrintWriter writer = resp.getWriter();
+writer.println(str);
+writer.println(tag);
+}
+public String getDescription() {
+return "simple test of field assignment";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100055, Requested 361. Please try again in 6m0.116999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly uses user input (the "name" parameter from the HTTP request) without any validation or sanitization, and then prints it out, making it vulnerable to a potential Cross-Site Scripting (XSS) attack. Additionally, the getTag() method is supposed to return the "tag" field, but it is currently returning the "str" field, which could also lead to security issues if the tag is used for security-related purposes.</t>
         </is>
       </c>
     </row>
@@ -1816,12 +3803,45 @@
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.datastructures;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Datastructures2 extends BasicTestCase implements MicroTestCase {
+public class C {
+private String str;
+public String getData(){return this.str;}
+public String getTag(){return this.str;}
+public void setData(String str){this.str = str;}
+}
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+C c1 = new C();
+c1.setData("def");
+C c2 = new C();
+c2.setData(name);
+String str1 = c1.getData();
+String str2 = c2.getData();
+PrintWriter writer = resp.getWriter();
+writer.println(str1);
+writer.println(str2);
+}
+public String getDescription() {
+return "simple test of field assignment";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100055, Requested 365. Please try again in 6m3.48s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a security vulnerability because it directly uses user input (the "name" parameter from the HTTP request) without proper validation or sanitization, and then prints it out as part of the response. This could potentially lead to a Cross-Site Scripting (XSS) attack if an attacker were to inject malicious code as the "name" parameter.</t>
         </is>
       </c>
     </row>
@@ -1833,12 +3853,45 @@
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.datastructures;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Datastructures3 extends BasicTestCase implements MicroTestCase {
+public class C {
+private String str;
+private C next;
+public String getData(){return this.str;}
+public void setData(String str){this.str = str;}
+public void setNext(C next){this.next = next;}
+}
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+C c1 = new C();
+c1.setData("anbc");
+C c2 = new C();
+c2.setData(name);
+c1.setNext(c2);
+String str = c1.next.str;
+PrintWriter writer = resp.getWriter();
+writer.println(str);
+}
+public String getDescription() {
+return "simple nexted data";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100055, Requested 358. Please try again in 5m57.348s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is vulnerable to a security vulnerability because it directly uses user input (the "name" parameter from the HTTP request) without proper validation or sanitization, and then prints it out as part of the response, making it susceptible to potential attacks such as cross-site scripting (XSS).</t>
         </is>
       </c>
     </row>
@@ -1850,12 +3903,45 @@
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.datastructures;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Datastructures4 extends BasicTestCase implements MicroTestCase {
+public class C {
+private String str;
+private C next;
+public String getData(){return this.str;}
+public void setData(String str){this.str = str;}
+public void setNext(C next){this.next = next;}
+}
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+C c1 = new C();
+c1.setData(name);
+C c2 = new C();
+c2.setData("abc");
+c1.setNext(c2);
+String str = c1.next.str;
+PrintWriter writer = resp.getWriter();
+writer.println(str);
+}
+public String getDescription() {
+return "simple nexted data";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100055, Requested 358. Please try again in 5m57.217s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly uses user input (the "name" parameter from the HTTP request) to set the data of an object (c1), and then uses this data to set the next object in the chain (c2). However, the actual vulnerability lies in the fact that the code then prints out the data of the next object (c2) which is "abc", but if the intention was to print the user input, it would be a vulnerability as it would allow an attacker to inject malicious data. But in this case, the code does not directly print the user input, instead, it prints a hardcoded string "abc". Nevertheless, the fact that user input is stored and used in the application flow poses a potential risk if this input is used elsewhere in the application in an unsafe manner.</t>
         </is>
       </c>
     </row>
@@ -1867,12 +3953,52 @@
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.datastructures;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Datastructures5 extends BasicTestCase implements MicroTestCase {
+public class C {
+private String str;
+private C next;
+public String getData(){return this.str;}
+public void setData(String str){this.str = str;}
+public void setNext(C next){this.next = next;}
+}
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+C c1 = new C();
+c1.setData("abc");
+C c2 = new C();
+c2.setData("def");
+c1.setNext(c2);
+C c3 = new C();
+c3.setData(name.toUpperCase());
+c2.setNext(c3);
+C c = c1;
+while (c != null) {
+String str = c.getData();
+PrintWriter writer = resp.getWriter();
+writer.println(str);
+c = c.next;
+}
+}
+public String getDescription() {
+return "nested data in a loop";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100055, Requested 386. Please try again in 6m21.279s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it directly uses user input (req.getParameter(FIELD_NAME)) without proper validation or sanitization, and then uses this input to construct a response (c3.setData(name.toUpperCase())). This could potentially lead to security issues such as cross-site scripting (XSS) if the input is not properly handled.</t>
         </is>
       </c>
     </row>
@@ -1884,760 +4010,51 @@
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
+          <t>package securibench.micro.datastructures;
+import java.io.IOException;
+import java.io.PrintWriter;
+import javax.servlet.http.HttpServletRequest;
+import javax.servlet.http.HttpServletResponse;
+import securibench.micro.BasicTestCase;
+import securibench.micro.MicroTestCase;
+public class Datastructures6 extends BasicTestCase implements MicroTestCase {
+public class C {
+private String str;
+private C next;
+public String getData(){return this.str;}
+public void setData(String str){this.str = str;}
+public void setNext(C next){this.next = next;}
+}
+private static final String FIELD_NAME = "name";
+protected void doGet(HttpServletRequest req, HttpServletResponse resp) throws IOException {
+String name = req.getParameter(FIELD_NAME);
+C c = new C();
+C head = c;
+for(int i = 0; i &lt; 1600; i++){
+C next = new C();
+c.setNext(next);
+c = next;
+}
+c.setData(name);
+c = head;
+while(c != null) {
+PrintWriter writer = resp.getWriter();
+writer.println(c.getData());
+c = c.next;
+}
+}
+public String getDescription() {
+return "nested data in a loop";
+}
+public int getVulnerabilityCount() {
+return 1;
+}
+}</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
         <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100055, Requested 374. Please try again in 6m10.764s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="3" t="inlineStr">
-        <is>
-          <t>factories\Factories1.java</t>
-        </is>
-      </c>
-      <c r="B84" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C84" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100054, Requested 292. Please try again in 4m59.741999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="3" t="inlineStr">
-        <is>
-          <t>factories\Factories2.java</t>
-        </is>
-      </c>
-      <c r="B85" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C85" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100054, Requested 291. Please try again in 4m58.715s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="3" t="inlineStr">
-        <is>
-          <t>factories\Factories3.java</t>
-        </is>
-      </c>
-      <c r="B86" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C86" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100054, Requested 338. Please try again in 5m39.177s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="3" t="inlineStr">
-        <is>
-          <t>inter\Inter1.java</t>
-        </is>
-      </c>
-      <c r="B87" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C87" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100054, Requested 306. Please try again in 5m11.335s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="3" t="inlineStr">
-        <is>
-          <t>inter\Inter10.java</t>
-        </is>
-      </c>
-      <c r="B88" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C88" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100054, Requested 318. Please try again in 5m21.559s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="3" t="inlineStr">
-        <is>
-          <t>inter\Inter11.java</t>
-        </is>
-      </c>
-      <c r="B89" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C89" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100053, Requested 331. Please try again in 5m32.597s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="3" t="inlineStr">
-        <is>
-          <t>inter\Inter12.java</t>
-        </is>
-      </c>
-      <c r="B90" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C90" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100053, Requested 384. Please try again in 6m18.253s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="3" t="inlineStr">
-        <is>
-          <t>inter\Inter13.java</t>
-        </is>
-      </c>
-      <c r="B91" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C91" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100053, Requested 320. Please try again in 5m22.798s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="3" t="inlineStr">
-        <is>
-          <t>inter\Inter14.java</t>
-        </is>
-      </c>
-      <c r="B92" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C92" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100053, Requested 334. Please try again in 5m34.756s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="3" t="inlineStr">
-        <is>
-          <t>inter\Inter2.java</t>
-        </is>
-      </c>
-      <c r="B93" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C93" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100053, Requested 321. Please try again in 5m23.373s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="3" t="inlineStr">
-        <is>
-          <t>inter\Inter3.java</t>
-        </is>
-      </c>
-      <c r="B94" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C94" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100053, Requested 441. Please try again in 7m6.895s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="3" t="inlineStr">
-        <is>
-          <t>inter\Inter4.java</t>
-        </is>
-      </c>
-      <c r="B95" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C95" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100052, Requested 310. Please try again in 5m13.349999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="3" t="inlineStr">
-        <is>
-          <t>inter\Inter5.java</t>
-        </is>
-      </c>
-      <c r="B96" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C96" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100052, Requested 314. Please try again in 5m16.642s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="3" t="inlineStr">
-        <is>
-          <t>inter\Inter6.java</t>
-        </is>
-      </c>
-      <c r="B97" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C97" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100052, Requested 309. Please try again in 5m12.127s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="3" t="inlineStr">
-        <is>
-          <t>inter\Inter7.java</t>
-        </is>
-      </c>
-      <c r="B98" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C98" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100052, Requested 365. Please try again in 6m0.357s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="3" t="inlineStr">
-        <is>
-          <t>inter\Inter8.java</t>
-        </is>
-      </c>
-      <c r="B99" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C99" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100051, Requested 352. Please try again in 5m48.978s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="3" t="inlineStr">
-        <is>
-          <t>inter\Inter9.java</t>
-        </is>
-      </c>
-      <c r="B100" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C100" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100051, Requested 355. Please try again in 5m51.376s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="3" t="inlineStr">
-        <is>
-          <t>pred\Pred1.java</t>
-        </is>
-      </c>
-      <c r="B101" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C101" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100051, Requested 282. Please try again in 4m48.061s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="3" t="inlineStr">
-        <is>
-          <t>pred\Pred2.java</t>
-        </is>
-      </c>
-      <c r="B102" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C102" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100051, Requested 307. Please try again in 5m9.498999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="3" t="inlineStr">
-        <is>
-          <t>pred\Pred3.java</t>
-        </is>
-      </c>
-      <c r="B103" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C103" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100051, Requested 307. Please try again in 5m9.318s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="3" t="inlineStr">
-        <is>
-          <t>pred\Pred4.java</t>
-        </is>
-      </c>
-      <c r="B104" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C104" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100050, Requested 288. Please try again in 4m52.737s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="3" t="inlineStr">
-        <is>
-          <t>pred\Pred5.java</t>
-        </is>
-      </c>
-      <c r="B105" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C105" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100050, Requested 299. Please try again in 5m2.069s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="3" t="inlineStr">
-        <is>
-          <t>pred\Pred6.java</t>
-        </is>
-      </c>
-      <c r="B106" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C106" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100050, Requested 288. Please try again in 4m52.312s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="3" t="inlineStr">
-        <is>
-          <t>pred\Pred7.java</t>
-        </is>
-      </c>
-      <c r="B107" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C107" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100050, Requested 296. Please try again in 4m59.01s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="3" t="inlineStr">
-        <is>
-          <t>pred\Pred8.java</t>
-        </is>
-      </c>
-      <c r="B108" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C108" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100049, Requested 302. Please try again in 5m4.037999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="3" t="inlineStr">
-        <is>
-          <t>pred\Pred9.java</t>
-        </is>
-      </c>
-      <c r="B109" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C109" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100049, Requested 302. Please try again in 5m3.882s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="3" t="inlineStr">
-        <is>
-          <t>reflection\Refl1.java</t>
-        </is>
-      </c>
-      <c r="B110" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C110" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100049, Requested 468. Please try again in 7m27.107999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="3" t="inlineStr">
-        <is>
-          <t>reflection\Refl2.java</t>
-        </is>
-      </c>
-      <c r="B111" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C111" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100049, Requested 398. Please try again in 6m26.515s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="3" t="inlineStr">
-        <is>
-          <t>reflection\Refl3.java</t>
-        </is>
-      </c>
-      <c r="B112" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C112" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100049, Requested 472. Please try again in 7m30.292s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="3" t="inlineStr">
-        <is>
-          <t>reflection\Refl4.java</t>
-        </is>
-      </c>
-      <c r="B113" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C113" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100048, Requested 363. Please try again in 5m55.921999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="3" t="inlineStr">
-        <is>
-          <t>sanitizers\Sanitizers1.java</t>
-        </is>
-      </c>
-      <c r="B114" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C114" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100048, Requested 434. Please try again in 6m57.055s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="3" t="inlineStr">
-        <is>
-          <t>sanitizers\Sanitizers2.java</t>
-        </is>
-      </c>
-      <c r="B115" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C115" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100048, Requested 412. Please try again in 6m37.893s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="3" t="inlineStr">
-        <is>
-          <t>sanitizers\Sanitizers3.java</t>
-        </is>
-      </c>
-      <c r="B116" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C116" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100048, Requested 295. Please try again in 4m56.628999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="3" t="inlineStr">
-        <is>
-          <t>sanitizers\Sanitizers4.java</t>
-        </is>
-      </c>
-      <c r="B117" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C117" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100048, Requested 380. Please try again in 6m9.894s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="3" t="inlineStr">
-        <is>
-          <t>sanitizers\Sanitizers5.java</t>
-        </is>
-      </c>
-      <c r="B118" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C118" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100047, Requested 327. Please try again in 5m23.958s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="3" t="inlineStr">
-        <is>
-          <t>sanitizers\Sanitizers6.java</t>
-        </is>
-      </c>
-      <c r="B119" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C119" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100047, Requested 417. Please try again in 6m41.561999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="3" t="inlineStr">
-        <is>
-          <t>session\Session1.java</t>
-        </is>
-      </c>
-      <c r="B120" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C120" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100047, Requested 320. Please try again in 5m17.595s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="3" t="inlineStr">
-        <is>
-          <t>session\Session2.java</t>
-        </is>
-      </c>
-      <c r="B121" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C121" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100047, Requested 342. Please try again in 5m36.434999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="3" t="inlineStr">
-        <is>
-          <t>session\Session3.java</t>
-        </is>
-      </c>
-      <c r="B122" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C122" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100047, Requested 364. Please try again in 5m55.313999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="3" t="inlineStr">
-        <is>
-          <t>strong_updates\StrongUpdates1.java</t>
-        </is>
-      </c>
-      <c r="B123" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C123" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100047, Requested 288. Please try again in 4m49.477999999s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="3" t="inlineStr">
-        <is>
-          <t>strong_updates\StrongUpdates2.java</t>
-        </is>
-      </c>
-      <c r="B124" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C124" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100046, Requested 288. Please try again in 4m49.328s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="3" t="inlineStr">
-        <is>
-          <t>strong_updates\StrongUpdates3.java</t>
-        </is>
-      </c>
-      <c r="B125" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C125" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100046, Requested 311. Please try again in 5m9.036s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="3" t="inlineStr">
-        <is>
-          <t>strong_updates\StrongUpdates4.java</t>
-        </is>
-      </c>
-      <c r="B126" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C126" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100046, Requested 313. Please try again in 5m10.574s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="3" t="inlineStr">
-        <is>
-          <t>strong_updates\StrongUpdates5.java</t>
-        </is>
-      </c>
-      <c r="B127" s="3" t="inlineStr">
-        <is>
-          <t>Erro durante a leitura ou processamento do arquivo.</t>
-        </is>
-      </c>
-      <c r="C127" s="3" t="inlineStr">
-        <is>
-          <t>Erro: Error code: 429 - {'error': {'message': 'Rate limit reached for model `llama-3.3-70b-versatile` in organization `org_01jva2j07sfeqshwj2rj357wr0` service tier `on_demand` on tokens per day (TPD): Limit 100000, Used 100046, Requested 302. Please try again in 5m0.94s. Need more tokens? Upgrade to Dev Tier today at https://console.groq.com/settings/billing', 'type': 'tokens', 'code': 'rate_limit_exceeded'}}</t>
+          <t>vulnerability: YES | vulnerability type: N/A | vulnerability name: N/A | explanation: The code snippet is subject to a security vulnerability because it is vulnerable to a null pointer exception and also it can be used for a potential denial of service (DoS) attack by providing a large input that can cause the loop to run indefinitely, but the main issue here is that it seems to be trying to simulate a linked list and print out the data in each node, however, in the while loop, it is trying to access c.next instead of c.getNext() which will cause a null pointer exception because 'next' is not a public field and cannot be accessed directly, also the getWriter() is called in a loop which can lead to unexpected behavior.</t>
         </is>
       </c>
     </row>

</xml_diff>